<commit_message>
fixed run_rothc_residue runs, which are now correctly calculated
</commit_message>
<xml_diff>
--- a/data/crops/rothc_support/annual_crops_rothc_scenarios.xlsx
+++ b/data/crops/rothc_support/annual_crops_rothc_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/rothc_support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF128BA2-775D-48AD-A9C8-4F2E648D042D}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7E12E4A-3422-4759-B616-5AFDABFFD2E3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F94B64D-243B-49DA-AE87-045B34BFAB0F}"/>
   </bookViews>
@@ -2054,7 +2054,7 @@
   <dimension ref="A1:T46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2207,7 +2207,7 @@
         <v>90</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G46" si="0">+"RothC results for year 2030 for "&amp;A3&amp;"_"&amp;D3&amp;" in ton C/ha"</f>
+        <f>+"RothC results for year 2030 for "&amp;A3&amp;"_"&amp;D3&amp;" in ton C/ha"</f>
         <v>RothC results for year 2030 for Barley_irr_roff in ton C/ha</v>
       </c>
       <c r="H3" t="s">
@@ -2264,7 +2264,7 @@
         <v>90</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G3:G46" si="0">+"RothC results for year 2030 for "&amp;A4&amp;"_"&amp;D4&amp;" in ton C/ha"</f>
         <v>RothC results for year 2030 for Cabbage_irr in ton C/ha</v>
       </c>
       <c r="H4" t="s">
@@ -4635,6 +4635,7 @@
   </sheetData>
   <autoFilter ref="A1:T46" xr:uid="{A1821CC5-2977-4A1A-B60B-8C004F05C4AF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>